<commit_message>
update from_to distance matrix; update ETL scripts
</commit_message>
<xml_diff>
--- a/input_data/oc_site.xlsx
+++ b/input_data/oc_site.xlsx
@@ -1,25 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jolene\Documents\Sumit\ProductDevelopment\haversine_distance\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jolene\GoogleDrive\Personal\Study\phd\model\workdir\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75808E9F-E347-4786-B5A3-F361B158CE6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE700677-7BC4-4DF1-9A00-0AE549725E57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{6FE78FDE-FEA8-4741-9142-6B1CDDCD843D}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="3" xr2:uid="{6FE78FDE-FEA8-4741-9142-6B1CDDCD843D}"/>
   </bookViews>
   <sheets>
-    <sheet name="sites" sheetId="1" r:id="rId1"/>
-    <sheet name="oc_site" sheetId="2" r:id="rId2"/>
+    <sheet name="sites" sheetId="1" state="hidden" r:id="rId1"/>
+    <sheet name="oc_site" sheetId="2" state="hidden" r:id="rId2"/>
     <sheet name="oc" sheetId="3" r:id="rId3"/>
+    <sheet name="pu" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">oc!$A$1:$T$443</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">oc_site!$A$1:$H$186</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">pu!$A$1:$D$29</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">sites!$A$1:$D$44</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6947" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6951" uniqueCount="668">
   <si>
     <t>RFY</t>
   </si>
@@ -2032,6 +2034,18 @@
   </si>
   <si>
     <t>blanks</t>
+  </si>
+  <si>
+    <t>ha</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -2075,7 +2089,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2086,6 +2100,18 @@
       <patternFill patternType="solid">
         <fgColor theme="3" tint="-0.249977111117893"/>
         <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -2110,7 +2136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2128,6 +2154,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2922,7 +2951,15 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7CF8E2B7-6414-4CED-AB45-997B5FBA320B}" name="Table2" displayName="Table2" ref="A1:H186" totalsRowShown="0" headerRowDxfId="31" headerRowBorderDxfId="30">
-  <autoFilter ref="A1:H186" xr:uid="{2248A905-F066-456D-8E71-C1972624B358}"/>
+  <autoFilter ref="A1:H186" xr:uid="{2248A905-F066-456D-8E71-C1972624B358}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Newgrow"/>
+        <filter val="Roepersfontein"/>
+        <filter val="Yarona"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{18E38F56-BA84-47A5-81F5-574A222B78AF}" name="location" dataDxfId="29"/>
     <tableColumn id="2" xr3:uid="{87FFD94F-28DC-4888-B8A8-DA7E01C4AD3F}" name="fc name" dataDxfId="28"/>
@@ -2941,11 +2978,7 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F7CFEB77-1983-4546-AEBD-D47F07FEA1F4}" name="Table1" displayName="Table1" ref="A1:X443" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
-  <autoFilter ref="A1:X443" xr:uid="{BE185733-7823-4470-AD92-9C8384CFB6FE}">
-    <filterColumn colId="21">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:X443" xr:uid="{BE185733-7823-4470-AD92-9C8384CFB6FE}"/>
   <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{14C393BA-A71A-4929-9889-415868BB3374}" name="ORCHARD" dataDxfId="23"/>
     <tableColumn id="2" xr3:uid="{FFE7F048-2425-4C5D-8685-966D0E99C041}" name="ORCHARDSECTION" dataDxfId="22"/>
@@ -3829,10 +3862,10 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9.88671875" customWidth="1"/>
-    <col min="2" max="2" width="21.21875" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
     <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="23.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" style="6" customWidth="1"/>
     <col min="6" max="6" width="17.88671875" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.5546875" bestFit="1" customWidth="1"/>
@@ -3864,7 +3897,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>90</v>
       </c>
@@ -3891,7 +3924,7 @@
         <v>20.12575</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>90</v>
       </c>
@@ -3918,7 +3951,7 @@
         <v>20.130040000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>90</v>
       </c>
@@ -3945,7 +3978,7 @@
         <v>20.13439</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>90</v>
       </c>
@@ -3972,7 +4005,7 @@
         <v>20.140129999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>90</v>
       </c>
@@ -3999,7 +4032,7 @@
         <v>20.140920000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>90</v>
       </c>
@@ -4026,7 +4059,7 @@
         <v>20.141739999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>90</v>
       </c>
@@ -4053,7 +4086,7 @@
         <v>20.148260000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>90</v>
       </c>
@@ -4080,7 +4113,7 @@
         <v>20.14799</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>90</v>
       </c>
@@ -4107,7 +4140,7 @@
         <v>20.075040000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>90</v>
       </c>
@@ -4134,7 +4167,7 @@
         <v>20.070730000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>90</v>
       </c>
@@ -4161,7 +4194,7 @@
         <v>20.070653979999999</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>90</v>
       </c>
@@ -4188,7 +4221,7 @@
         <v>20.07055901</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>90</v>
       </c>
@@ -4215,7 +4248,7 @@
         <v>20.070419999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>90</v>
       </c>
@@ -4242,7 +4275,7 @@
         <v>20.067530000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>90</v>
       </c>
@@ -4269,7 +4302,7 @@
         <v>20.070640000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>90</v>
       </c>
@@ -4296,7 +4329,7 @@
         <v>20.06737</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>90</v>
       </c>
@@ -4323,7 +4356,7 @@
         <v>20.067620000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>90</v>
       </c>
@@ -4350,7 +4383,7 @@
         <v>20.038</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>90</v>
       </c>
@@ -4377,7 +4410,7 @@
         <v>20.042549999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>90</v>
       </c>
@@ -4404,7 +4437,7 @@
         <v>20.04513</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>90</v>
       </c>
@@ -4431,7 +4464,7 @@
         <v>19.993310000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>90</v>
       </c>
@@ -4458,7 +4491,7 @@
         <v>19.995519999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>90</v>
       </c>
@@ -4485,7 +4518,7 @@
         <v>19.9876</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>90</v>
       </c>
@@ -4512,7 +4545,7 @@
         <v>19.98799</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>90</v>
       </c>
@@ -4539,7 +4572,7 @@
         <v>19.992180000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>90</v>
       </c>
@@ -4566,7 +4599,7 @@
         <v>19.987410000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>90</v>
       </c>
@@ -4593,7 +4626,7 @@
         <v>19.995049999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>90</v>
       </c>
@@ -4620,7 +4653,7 @@
         <v>19.987570000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>125</v>
       </c>
@@ -4647,7 +4680,7 @@
         <v>20.79271</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>125</v>
       </c>
@@ -4674,7 +4707,7 @@
         <v>20.787600000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>125</v>
       </c>
@@ -4701,7 +4734,7 @@
         <v>20.783539999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>125</v>
       </c>
@@ -4728,7 +4761,7 @@
         <v>20.780819999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>125</v>
       </c>
@@ -4755,7 +4788,7 @@
         <v>20.78022</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>125</v>
       </c>
@@ -4782,7 +4815,7 @@
         <v>20.79156</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>125</v>
       </c>
@@ -4809,7 +4842,7 @@
         <v>20.795390000000001</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>125</v>
       </c>
@@ -4836,7 +4869,7 @@
         <v>20.79156</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>125</v>
       </c>
@@ -4863,7 +4896,7 @@
         <v>20.79476</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>125</v>
       </c>
@@ -4890,7 +4923,7 @@
         <v>20.791840000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>125</v>
       </c>
@@ -4917,7 +4950,7 @@
         <v>20.791679999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>125</v>
       </c>
@@ -4944,7 +4977,7 @@
         <v>20.786380000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>125</v>
       </c>
@@ -4971,7 +5004,7 @@
         <v>20.784500000000001</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>125</v>
       </c>
@@ -4998,7 +5031,7 @@
         <v>20.787379999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>125</v>
       </c>
@@ -5025,7 +5058,7 @@
         <v>20.42098</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>125</v>
       </c>
@@ -5052,7 +5085,7 @@
         <v>20.785229999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>125</v>
       </c>
@@ -5079,7 +5112,7 @@
         <v>20.786069999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>125</v>
       </c>
@@ -5106,7 +5139,7 @@
         <v>20.78492</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>125</v>
       </c>
@@ -5133,7 +5166,7 @@
         <v>20.783519999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>125</v>
       </c>
@@ -5160,7 +5193,7 @@
         <v>20.780750000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>125</v>
       </c>
@@ -5187,7 +5220,7 @@
         <v>20.786999999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>125</v>
       </c>
@@ -5214,7 +5247,7 @@
         <v>20.785049999999998</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>125</v>
       </c>
@@ -5241,7 +5274,7 @@
         <v>20.659839999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>125</v>
       </c>
@@ -5268,7 +5301,7 @@
         <v>20.657530000000001</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>125</v>
       </c>
@@ -5295,7 +5328,7 @@
         <v>20.654820000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>125</v>
       </c>
@@ -5322,7 +5355,7 @@
         <v>20.655360000000002</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>125</v>
       </c>
@@ -5349,7 +5382,7 @@
         <v>20.656490000000002</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>125</v>
       </c>
@@ -5376,7 +5409,7 @@
         <v>20.659410000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>125</v>
       </c>
@@ -5403,7 +5436,7 @@
         <v>20.655760000000001</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>125</v>
       </c>
@@ -5430,7 +5463,7 @@
         <v>20.657219999999999</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>125</v>
       </c>
@@ -5457,7 +5490,7 @@
         <v>20.655059999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>125</v>
       </c>
@@ -5484,7 +5517,7 @@
         <v>20.65907</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>125</v>
       </c>
@@ -5511,7 +5544,7 @@
         <v>20.658180000000002</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>125</v>
       </c>
@@ -5538,7 +5571,7 @@
         <v>20.656669999999998</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>125</v>
       </c>
@@ -5565,7 +5598,7 @@
         <v>20.65408</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>125</v>
       </c>
@@ -5592,7 +5625,7 @@
         <v>20.636710000000001</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>125</v>
       </c>
@@ -5619,7 +5652,7 @@
         <v>20.65587</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>125</v>
       </c>
@@ -5646,7 +5679,7 @@
         <v>20.655529999999999</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>125</v>
       </c>
@@ -5673,7 +5706,7 @@
         <v>20.65399</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>125</v>
       </c>
@@ -5700,7 +5733,7 @@
         <v>20.654520000000002</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>125</v>
       </c>
@@ -5727,7 +5760,7 @@
         <v>20.652850000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>125</v>
       </c>
@@ -5754,7 +5787,7 @@
         <v>20.643039999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>125</v>
       </c>
@@ -5781,7 +5814,7 @@
         <v>20.646129999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>125</v>
       </c>
@@ -5808,7 +5841,7 @@
         <v>20.656669999999998</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>125</v>
       </c>
@@ -5835,7 +5868,7 @@
         <v>20.676210000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>125</v>
       </c>
@@ -5862,7 +5895,7 @@
         <v>20.673649999999999</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>125</v>
       </c>
@@ -5889,7 +5922,7 @@
         <v>20.676100000000002</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>125</v>
       </c>
@@ -5916,7 +5949,7 @@
         <v>20.673960000000001</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>125</v>
       </c>
@@ -5943,7 +5976,7 @@
         <v>20.656700000000001</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>125</v>
       </c>
@@ -5970,7 +6003,7 @@
         <v>20.659610000000001</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>125</v>
       </c>
@@ -5997,7 +6030,7 @@
         <v>20.65503</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>125</v>
       </c>
@@ -6024,7 +6057,7 @@
         <v>20.650749999999999</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>125</v>
       </c>
@@ -6051,7 +6084,7 @@
         <v>20.650929999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>125</v>
       </c>
@@ -6078,7 +6111,7 @@
         <v>20.641100000000002</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>125</v>
       </c>
@@ -6105,7 +6138,7 @@
         <v>20.641120000000001</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>125</v>
       </c>
@@ -6132,7 +6165,7 @@
         <v>20.641079999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>125</v>
       </c>
@@ -6159,7 +6192,7 @@
         <v>20.653639999999999</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>125</v>
       </c>
@@ -6186,7 +6219,7 @@
         <v>20.636649999999999</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>125</v>
       </c>
@@ -6213,7 +6246,7 @@
         <v>20.65691</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>125</v>
       </c>
@@ -6240,7 +6273,7 @@
         <v>20.63897</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>125</v>
       </c>
@@ -6267,7 +6300,7 @@
         <v>20.638839999999998</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>125</v>
       </c>
@@ -6294,7 +6327,7 @@
         <v>20.653279999999999</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>125</v>
       </c>
@@ -6321,7 +6354,7 @@
         <v>20.64143</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>125</v>
       </c>
@@ -6348,7 +6381,7 @@
         <v>20.64461</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>125</v>
       </c>
@@ -6375,7 +6408,7 @@
         <v>20.64622</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>125</v>
       </c>
@@ -6402,7 +6435,7 @@
         <v>20.6571</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>125</v>
       </c>
@@ -6429,7 +6462,7 @@
         <v>20.648990000000001</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>125</v>
       </c>
@@ -6456,7 +6489,7 @@
         <v>20.647749999999998</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>125</v>
       </c>
@@ -6483,7 +6516,7 @@
         <v>20.646940000000001</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>125</v>
       </c>
@@ -6510,7 +6543,7 @@
         <v>20.65</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>125</v>
       </c>
@@ -6537,7 +6570,7 @@
         <v>20.647189999999998</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>125</v>
       </c>
@@ -6564,7 +6597,7 @@
         <v>20.64292</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>125</v>
       </c>
@@ -6591,7 +6624,7 @@
         <v>20.645009999999999</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>125</v>
       </c>
@@ -6618,7 +6651,7 @@
         <v>20.642959999999999</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
         <v>125</v>
       </c>
@@ -8871,8 +8904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0F7152E-70A5-4EEF-A05A-76F02DC07F2C}">
   <dimension ref="A1:X443"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K368" workbookViewId="0">
-      <selection activeCell="X443" sqref="X443"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8974,7 +9007,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="2" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>289</v>
       </c>
@@ -9047,7 +9080,7 @@
       </c>
       <c r="X2" s="7"/>
     </row>
-    <row r="3" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>301</v>
       </c>
@@ -9120,7 +9153,7 @@
       </c>
       <c r="X3" s="7"/>
     </row>
-    <row r="4" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>305</v>
       </c>
@@ -9193,7 +9226,7 @@
       </c>
       <c r="X4" s="7"/>
     </row>
-    <row r="5" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>306</v>
       </c>
@@ -9266,7 +9299,7 @@
       </c>
       <c r="X5" s="7"/>
     </row>
-    <row r="6" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>307</v>
       </c>
@@ -9339,7 +9372,7 @@
       </c>
       <c r="X6" s="7"/>
     </row>
-    <row r="7" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>309</v>
       </c>
@@ -9412,7 +9445,7 @@
       </c>
       <c r="X7" s="7"/>
     </row>
-    <row r="8" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>310</v>
       </c>
@@ -9485,7 +9518,7 @@
       </c>
       <c r="X8" s="7"/>
     </row>
-    <row r="9" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>312</v>
       </c>
@@ -9558,7 +9591,7 @@
       </c>
       <c r="X9" s="7"/>
     </row>
-    <row r="10" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>313</v>
       </c>
@@ -9631,7 +9664,7 @@
       </c>
       <c r="X10" s="7"/>
     </row>
-    <row r="11" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>315</v>
       </c>
@@ -9704,7 +9737,7 @@
       </c>
       <c r="X11" s="7"/>
     </row>
-    <row r="12" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>317</v>
       </c>
@@ -9777,7 +9810,7 @@
       </c>
       <c r="X12" s="7"/>
     </row>
-    <row r="13" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>318</v>
       </c>
@@ -9850,7 +9883,7 @@
       </c>
       <c r="X13" s="7"/>
     </row>
-    <row r="14" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>319</v>
       </c>
@@ -9923,7 +9956,7 @@
       </c>
       <c r="X14" s="7"/>
     </row>
-    <row r="15" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>320</v>
       </c>
@@ -9996,7 +10029,7 @@
       </c>
       <c r="X15" s="7"/>
     </row>
-    <row r="16" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>323</v>
       </c>
@@ -10069,7 +10102,7 @@
       </c>
       <c r="X16" s="7"/>
     </row>
-    <row r="17" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>324</v>
       </c>
@@ -10142,7 +10175,7 @@
       </c>
       <c r="X17" s="7"/>
     </row>
-    <row r="18" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>325</v>
       </c>
@@ -10215,7 +10248,7 @@
       </c>
       <c r="X18" s="7"/>
     </row>
-    <row r="19" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>326</v>
       </c>
@@ -10288,7 +10321,7 @@
       </c>
       <c r="X19" s="7"/>
     </row>
-    <row r="20" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>327</v>
       </c>
@@ -10361,7 +10394,7 @@
       </c>
       <c r="X20" s="7"/>
     </row>
-    <row r="21" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>328</v>
       </c>
@@ -10434,7 +10467,7 @@
       </c>
       <c r="X21" s="7"/>
     </row>
-    <row r="22" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>329</v>
       </c>
@@ -10507,7 +10540,7 @@
       </c>
       <c r="X22" s="7"/>
     </row>
-    <row r="23" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>330</v>
       </c>
@@ -10580,7 +10613,7 @@
       </c>
       <c r="X23" s="7"/>
     </row>
-    <row r="24" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>332</v>
       </c>
@@ -10653,7 +10686,7 @@
       </c>
       <c r="X24" s="7"/>
     </row>
-    <row r="25" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>333</v>
       </c>
@@ -10726,7 +10759,7 @@
       </c>
       <c r="X25" s="7"/>
     </row>
-    <row r="26" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>335</v>
       </c>
@@ -10799,7 +10832,7 @@
       </c>
       <c r="X26" s="7"/>
     </row>
-    <row r="27" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>336</v>
       </c>
@@ -10872,7 +10905,7 @@
       </c>
       <c r="X27" s="7"/>
     </row>
-    <row r="28" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>337</v>
       </c>
@@ -10945,7 +10978,7 @@
       </c>
       <c r="X28" s="7"/>
     </row>
-    <row r="29" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>339</v>
       </c>
@@ -11018,7 +11051,7 @@
       </c>
       <c r="X29" s="7"/>
     </row>
-    <row r="30" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>340</v>
       </c>
@@ -11091,7 +11124,7 @@
       </c>
       <c r="X30" s="7"/>
     </row>
-    <row r="31" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>341</v>
       </c>
@@ -11164,7 +11197,7 @@
       </c>
       <c r="X31" s="7"/>
     </row>
-    <row r="32" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>342</v>
       </c>
@@ -11237,7 +11270,7 @@
       </c>
       <c r="X32" s="7"/>
     </row>
-    <row r="33" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>343</v>
       </c>
@@ -11310,7 +11343,7 @@
       </c>
       <c r="X33" s="7"/>
     </row>
-    <row r="34" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>344</v>
       </c>
@@ -11383,7 +11416,7 @@
       </c>
       <c r="X34" s="7"/>
     </row>
-    <row r="35" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>345</v>
       </c>
@@ -11456,7 +11489,7 @@
       </c>
       <c r="X35" s="7"/>
     </row>
-    <row r="36" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>346</v>
       </c>
@@ -11529,7 +11562,7 @@
       </c>
       <c r="X36" s="7"/>
     </row>
-    <row r="37" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>347</v>
       </c>
@@ -11602,7 +11635,7 @@
       </c>
       <c r="X37" s="7"/>
     </row>
-    <row r="38" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>348</v>
       </c>
@@ -11675,7 +11708,7 @@
       </c>
       <c r="X38" s="7"/>
     </row>
-    <row r="39" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>349</v>
       </c>
@@ -11748,7 +11781,7 @@
       </c>
       <c r="X39" s="7"/>
     </row>
-    <row r="40" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>350</v>
       </c>
@@ -11821,7 +11854,7 @@
       </c>
       <c r="X40" s="7"/>
     </row>
-    <row r="41" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>351</v>
       </c>
@@ -11894,7 +11927,7 @@
       </c>
       <c r="X41" s="7"/>
     </row>
-    <row r="42" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>292</v>
       </c>
@@ -11967,7 +12000,7 @@
       </c>
       <c r="X42" s="7"/>
     </row>
-    <row r="43" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>352</v>
       </c>
@@ -12040,7 +12073,7 @@
       </c>
       <c r="X43" s="7"/>
     </row>
-    <row r="44" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>353</v>
       </c>
@@ -12113,7 +12146,7 @@
       </c>
       <c r="X44" s="7"/>
     </row>
-    <row r="45" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>354</v>
       </c>
@@ -12186,7 +12219,7 @@
       </c>
       <c r="X45" s="7"/>
     </row>
-    <row r="46" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>356</v>
       </c>
@@ -12259,7 +12292,7 @@
       </c>
       <c r="X46" s="7"/>
     </row>
-    <row r="47" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>357</v>
       </c>
@@ -12332,7 +12365,7 @@
       </c>
       <c r="X47" s="7"/>
     </row>
-    <row r="48" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>358</v>
       </c>
@@ -12405,7 +12438,7 @@
       </c>
       <c r="X48" s="7"/>
     </row>
-    <row r="49" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>359</v>
       </c>
@@ -12478,7 +12511,7 @@
       </c>
       <c r="X49" s="7"/>
     </row>
-    <row r="50" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>360</v>
       </c>
@@ -12551,7 +12584,7 @@
       </c>
       <c r="X50" s="7"/>
     </row>
-    <row r="51" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>363</v>
       </c>
@@ -12624,7 +12657,7 @@
       </c>
       <c r="X51" s="7"/>
     </row>
-    <row r="52" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>364</v>
       </c>
@@ -12697,7 +12730,7 @@
       </c>
       <c r="X52" s="7"/>
     </row>
-    <row r="53" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>365</v>
       </c>
@@ -12770,7 +12803,7 @@
       </c>
       <c r="X53" s="7"/>
     </row>
-    <row r="54" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>366</v>
       </c>
@@ -12843,7 +12876,7 @@
       </c>
       <c r="X54" s="7"/>
     </row>
-    <row r="55" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>367</v>
       </c>
@@ -12916,7 +12949,7 @@
       </c>
       <c r="X55" s="7"/>
     </row>
-    <row r="56" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>368</v>
       </c>
@@ -12989,7 +13022,7 @@
       </c>
       <c r="X56" s="7"/>
     </row>
-    <row r="57" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>369</v>
       </c>
@@ -13062,7 +13095,7 @@
       </c>
       <c r="X57" s="7"/>
     </row>
-    <row r="58" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>370</v>
       </c>
@@ -13135,7 +13168,7 @@
       </c>
       <c r="X58" s="7"/>
     </row>
-    <row r="59" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>371</v>
       </c>
@@ -13208,7 +13241,7 @@
       </c>
       <c r="X59" s="7"/>
     </row>
-    <row r="60" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>372</v>
       </c>
@@ -13281,7 +13314,7 @@
       </c>
       <c r="X60" s="7"/>
     </row>
-    <row r="61" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
         <v>373</v>
       </c>
@@ -13354,7 +13387,7 @@
       </c>
       <c r="X61" s="7"/>
     </row>
-    <row r="62" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>374</v>
       </c>
@@ -13427,7 +13460,7 @@
       </c>
       <c r="X62" s="7"/>
     </row>
-    <row r="63" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>375</v>
       </c>
@@ -13500,7 +13533,7 @@
       </c>
       <c r="X63" s="7"/>
     </row>
-    <row r="64" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>376</v>
       </c>
@@ -13573,7 +13606,7 @@
       </c>
       <c r="X64" s="7"/>
     </row>
-    <row r="65" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>377</v>
       </c>
@@ -13646,7 +13679,7 @@
       </c>
       <c r="X65" s="7"/>
     </row>
-    <row r="66" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
         <v>379</v>
       </c>
@@ -13719,7 +13752,7 @@
       </c>
       <c r="X66" s="7"/>
     </row>
-    <row r="67" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
         <v>380</v>
       </c>
@@ -13792,7 +13825,7 @@
       </c>
       <c r="X67" s="7"/>
     </row>
-    <row r="68" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
         <v>381</v>
       </c>
@@ -13865,7 +13898,7 @@
       </c>
       <c r="X68" s="7"/>
     </row>
-    <row r="69" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
         <v>382</v>
       </c>
@@ -13938,7 +13971,7 @@
       </c>
       <c r="X69" s="7"/>
     </row>
-    <row r="70" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
         <v>383</v>
       </c>
@@ -14011,7 +14044,7 @@
       </c>
       <c r="X70" s="7"/>
     </row>
-    <row r="71" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
         <v>385</v>
       </c>
@@ -14084,7 +14117,7 @@
       </c>
       <c r="X71" s="7"/>
     </row>
-    <row r="72" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
         <v>387</v>
       </c>
@@ -14157,7 +14190,7 @@
       </c>
       <c r="X72" s="7"/>
     </row>
-    <row r="73" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
         <v>388</v>
       </c>
@@ -14230,7 +14263,7 @@
       </c>
       <c r="X73" s="7"/>
     </row>
-    <row r="74" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
         <v>390</v>
       </c>
@@ -14303,7 +14336,7 @@
       </c>
       <c r="X74" s="7"/>
     </row>
-    <row r="75" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
         <v>393</v>
       </c>
@@ -14376,7 +14409,7 @@
       </c>
       <c r="X75" s="7"/>
     </row>
-    <row r="76" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
         <v>394</v>
       </c>
@@ -14449,7 +14482,7 @@
       </c>
       <c r="X76" s="7"/>
     </row>
-    <row r="77" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
         <v>395</v>
       </c>
@@ -14522,7 +14555,7 @@
       </c>
       <c r="X77" s="7"/>
     </row>
-    <row r="78" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
         <v>397</v>
       </c>
@@ -14595,7 +14628,7 @@
       </c>
       <c r="X78" s="7"/>
     </row>
-    <row r="79" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
         <v>398</v>
       </c>
@@ -14668,7 +14701,7 @@
       </c>
       <c r="X79" s="7"/>
     </row>
-    <row r="80" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
         <v>401</v>
       </c>
@@ -14741,7 +14774,7 @@
       </c>
       <c r="X80" s="7"/>
     </row>
-    <row r="81" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
         <v>402</v>
       </c>
@@ -14814,7 +14847,7 @@
       </c>
       <c r="X81" s="7"/>
     </row>
-    <row r="82" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
         <v>403</v>
       </c>
@@ -14887,7 +14920,7 @@
       </c>
       <c r="X82" s="7"/>
     </row>
-    <row r="83" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
         <v>404</v>
       </c>
@@ -14960,7 +14993,7 @@
       </c>
       <c r="X83" s="7"/>
     </row>
-    <row r="84" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
         <v>407</v>
       </c>
@@ -15033,7 +15066,7 @@
       </c>
       <c r="X84" s="7"/>
     </row>
-    <row r="85" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
         <v>408</v>
       </c>
@@ -15181,7 +15214,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="87" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
         <v>412</v>
       </c>
@@ -15254,7 +15287,7 @@
       </c>
       <c r="X87" s="7"/>
     </row>
-    <row r="88" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
         <v>413</v>
       </c>
@@ -15327,7 +15360,7 @@
       </c>
       <c r="X88" s="7"/>
     </row>
-    <row r="89" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
         <v>414</v>
       </c>
@@ -15400,7 +15433,7 @@
       </c>
       <c r="X89" s="7"/>
     </row>
-    <row r="90" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
         <v>385</v>
       </c>
@@ -15473,7 +15506,7 @@
       </c>
       <c r="X90" s="7"/>
     </row>
-    <row r="91" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
         <v>415</v>
       </c>
@@ -15546,7 +15579,7 @@
       </c>
       <c r="X91" s="7"/>
     </row>
-    <row r="92" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
         <v>417</v>
       </c>
@@ -15619,7 +15652,7 @@
       </c>
       <c r="X92" s="7"/>
     </row>
-    <row r="93" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="s">
         <v>417</v>
       </c>
@@ -15692,7 +15725,7 @@
       </c>
       <c r="X93" s="7"/>
     </row>
-    <row r="94" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
         <v>418</v>
       </c>
@@ -16290,7 +16323,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="102" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A102" s="4" t="s">
         <v>425</v>
       </c>
@@ -16363,7 +16396,7 @@
       </c>
       <c r="X102" s="7"/>
     </row>
-    <row r="103" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A103" s="4" t="s">
         <v>426</v>
       </c>
@@ -16436,7 +16469,7 @@
       </c>
       <c r="X103" s="7"/>
     </row>
-    <row r="104" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
         <v>427</v>
       </c>
@@ -16509,7 +16542,7 @@
       </c>
       <c r="X104" s="7"/>
     </row>
-    <row r="105" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A105" s="4" t="s">
         <v>428</v>
       </c>
@@ -16657,7 +16690,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="107" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A107" s="4" t="s">
         <v>430</v>
       </c>
@@ -16730,7 +16763,7 @@
       </c>
       <c r="X107" s="7"/>
     </row>
-    <row r="108" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A108" s="4" t="s">
         <v>419</v>
       </c>
@@ -16803,7 +16836,7 @@
       </c>
       <c r="X108" s="7"/>
     </row>
-    <row r="109" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A109" s="4" t="s">
         <v>422</v>
       </c>
@@ -16876,7 +16909,7 @@
       </c>
       <c r="X109" s="7"/>
     </row>
-    <row r="110" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A110" s="4" t="s">
         <v>431</v>
       </c>
@@ -17099,7 +17132,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="113" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A113" s="4" t="s">
         <v>433</v>
       </c>
@@ -17247,7 +17280,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="115" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A115" s="4" t="s">
         <v>435</v>
       </c>
@@ -17320,7 +17353,7 @@
       </c>
       <c r="X115" s="7"/>
     </row>
-    <row r="116" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
         <v>436</v>
       </c>
@@ -17543,7 +17576,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="119" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A119" s="4" t="s">
         <v>439</v>
       </c>
@@ -17616,7 +17649,7 @@
       </c>
       <c r="X119" s="7"/>
     </row>
-    <row r="120" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A120" s="4" t="s">
         <v>440</v>
       </c>
@@ -17764,7 +17797,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="122" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A122" s="4" t="s">
         <v>372</v>
       </c>
@@ -17837,7 +17870,7 @@
       </c>
       <c r="X122" s="7"/>
     </row>
-    <row r="123" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A123" s="4" t="s">
         <v>443</v>
       </c>
@@ -17910,7 +17943,7 @@
       </c>
       <c r="X123" s="7"/>
     </row>
-    <row r="124" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A124" s="4" t="s">
         <v>386</v>
       </c>
@@ -17983,7 +18016,7 @@
       </c>
       <c r="X124" s="7"/>
     </row>
-    <row r="125" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A125" s="4" t="s">
         <v>445</v>
       </c>
@@ -18056,7 +18089,7 @@
       </c>
       <c r="X125" s="7"/>
     </row>
-    <row r="126" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A126" s="4" t="s">
         <v>317</v>
       </c>
@@ -18129,7 +18162,7 @@
       </c>
       <c r="X126" s="7"/>
     </row>
-    <row r="127" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A127" s="4" t="s">
         <v>365</v>
       </c>
@@ -18202,7 +18235,7 @@
       </c>
       <c r="X127" s="7"/>
     </row>
-    <row r="128" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A128" s="4" t="s">
         <v>366</v>
       </c>
@@ -18275,7 +18308,7 @@
       </c>
       <c r="X128" s="7"/>
     </row>
-    <row r="129" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A129" s="4" t="s">
         <v>328</v>
       </c>
@@ -18348,7 +18381,7 @@
       </c>
       <c r="X129" s="7"/>
     </row>
-    <row r="130" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A130" s="4" t="s">
         <v>327</v>
       </c>
@@ -18421,7 +18454,7 @@
       </c>
       <c r="X130" s="7"/>
     </row>
-    <row r="131" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A131" s="4" t="s">
         <v>289</v>
       </c>
@@ -18494,7 +18527,7 @@
       </c>
       <c r="X131" s="7"/>
     </row>
-    <row r="132" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A132" s="4" t="s">
         <v>446</v>
       </c>
@@ -18567,7 +18600,7 @@
       </c>
       <c r="X132" s="7"/>
     </row>
-    <row r="133" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A133" s="4" t="s">
         <v>447</v>
       </c>
@@ -18640,7 +18673,7 @@
       </c>
       <c r="X133" s="7"/>
     </row>
-    <row r="134" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A134" s="4" t="s">
         <v>448</v>
       </c>
@@ -18713,7 +18746,7 @@
       </c>
       <c r="X134" s="7"/>
     </row>
-    <row r="135" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A135" s="4" t="s">
         <v>449</v>
       </c>
@@ -18786,7 +18819,7 @@
       </c>
       <c r="X135" s="7"/>
     </row>
-    <row r="136" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A136" s="4" t="s">
         <v>450</v>
       </c>
@@ -18859,7 +18892,7 @@
       </c>
       <c r="X136" s="7"/>
     </row>
-    <row r="137" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A137" s="4" t="s">
         <v>312</v>
       </c>
@@ -18932,7 +18965,7 @@
       </c>
       <c r="X137" s="7"/>
     </row>
-    <row r="138" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A138" s="4" t="s">
         <v>453</v>
       </c>
@@ -19005,7 +19038,7 @@
       </c>
       <c r="X138" s="7"/>
     </row>
-    <row r="139" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A139" s="4" t="s">
         <v>454</v>
       </c>
@@ -19078,7 +19111,7 @@
       </c>
       <c r="X139" s="7"/>
     </row>
-    <row r="140" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A140" s="4" t="s">
         <v>313</v>
       </c>
@@ -19151,7 +19184,7 @@
       </c>
       <c r="X140" s="7"/>
     </row>
-    <row r="141" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A141" s="4" t="s">
         <v>356</v>
       </c>
@@ -19224,7 +19257,7 @@
       </c>
       <c r="X141" s="7"/>
     </row>
-    <row r="142" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A142" s="4" t="s">
         <v>363</v>
       </c>
@@ -19297,7 +19330,7 @@
       </c>
       <c r="X142" s="7"/>
     </row>
-    <row r="143" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A143" s="4" t="s">
         <v>455</v>
       </c>
@@ -19370,7 +19403,7 @@
       </c>
       <c r="X143" s="7"/>
     </row>
-    <row r="144" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A144" s="4" t="s">
         <v>456</v>
       </c>
@@ -19443,7 +19476,7 @@
       </c>
       <c r="X144" s="7"/>
     </row>
-    <row r="145" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A145" s="4" t="s">
         <v>446</v>
       </c>
@@ -19516,7 +19549,7 @@
       </c>
       <c r="X145" s="7"/>
     </row>
-    <row r="146" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A146" s="4" t="s">
         <v>447</v>
       </c>
@@ -19589,7 +19622,7 @@
       </c>
       <c r="X146" s="7"/>
     </row>
-    <row r="147" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A147" s="4" t="s">
         <v>360</v>
       </c>
@@ -19662,7 +19695,7 @@
       </c>
       <c r="X147" s="7"/>
     </row>
-    <row r="148" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A148" s="4" t="s">
         <v>457</v>
       </c>
@@ -19735,7 +19768,7 @@
       </c>
       <c r="X148" s="7"/>
     </row>
-    <row r="149" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A149" s="4" t="s">
         <v>458</v>
       </c>
@@ -19808,7 +19841,7 @@
       </c>
       <c r="X149" s="7"/>
     </row>
-    <row r="150" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A150" s="4" t="s">
         <v>459</v>
       </c>
@@ -19881,7 +19914,7 @@
       </c>
       <c r="X150" s="7"/>
     </row>
-    <row r="151" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A151" s="4" t="s">
         <v>380</v>
       </c>
@@ -19954,7 +19987,7 @@
       </c>
       <c r="X151" s="7"/>
     </row>
-    <row r="152" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A152" s="4" t="s">
         <v>460</v>
       </c>
@@ -20027,7 +20060,7 @@
       </c>
       <c r="X152" s="7"/>
     </row>
-    <row r="153" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A153" s="4" t="s">
         <v>461</v>
       </c>
@@ -20100,7 +20133,7 @@
       </c>
       <c r="X153" s="7"/>
     </row>
-    <row r="154" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A154" s="4" t="s">
         <v>462</v>
       </c>
@@ -20173,7 +20206,7 @@
       </c>
       <c r="X154" s="7"/>
     </row>
-    <row r="155" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A155" s="4" t="s">
         <v>463</v>
       </c>
@@ -20246,7 +20279,7 @@
       </c>
       <c r="X155" s="7"/>
     </row>
-    <row r="156" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A156" s="4" t="s">
         <v>464</v>
       </c>
@@ -20319,7 +20352,7 @@
       </c>
       <c r="X156" s="7"/>
     </row>
-    <row r="157" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A157" s="4" t="s">
         <v>408</v>
       </c>
@@ -20392,7 +20425,7 @@
       </c>
       <c r="X157" s="7"/>
     </row>
-    <row r="158" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A158" s="4" t="s">
         <v>465</v>
       </c>
@@ -20465,7 +20498,7 @@
       </c>
       <c r="X158" s="7"/>
     </row>
-    <row r="159" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A159" s="4" t="s">
         <v>466</v>
       </c>
@@ -20538,7 +20571,7 @@
       </c>
       <c r="X159" s="7"/>
     </row>
-    <row r="160" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A160" s="4" t="s">
         <v>467</v>
       </c>
@@ -20836,7 +20869,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="164" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A164" s="4" t="s">
         <v>428</v>
       </c>
@@ -20909,7 +20942,7 @@
       </c>
       <c r="X164" s="7"/>
     </row>
-    <row r="165" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A165" s="4" t="s">
         <v>469</v>
       </c>
@@ -20982,7 +21015,7 @@
       </c>
       <c r="X165" s="7"/>
     </row>
-    <row r="166" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A166" s="4" t="s">
         <v>465</v>
       </c>
@@ -21055,7 +21088,7 @@
       </c>
       <c r="X166" s="7"/>
     </row>
-    <row r="167" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A167" s="4" t="s">
         <v>470</v>
       </c>
@@ -21128,7 +21161,7 @@
       </c>
       <c r="X167" s="7"/>
     </row>
-    <row r="168" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A168" s="4" t="s">
         <v>471</v>
       </c>
@@ -21201,7 +21234,7 @@
       </c>
       <c r="X168" s="7"/>
     </row>
-    <row r="169" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A169" s="4" t="s">
         <v>472</v>
       </c>
@@ -21349,7 +21382,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="171" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A171" s="4" t="s">
         <v>474</v>
       </c>
@@ -21422,7 +21455,7 @@
       </c>
       <c r="X171" s="7"/>
     </row>
-    <row r="172" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A172" s="4" t="s">
         <v>475</v>
       </c>
@@ -21495,7 +21528,7 @@
       </c>
       <c r="X172" s="7"/>
     </row>
-    <row r="173" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A173" s="4" t="s">
         <v>476</v>
       </c>
@@ -21568,7 +21601,7 @@
       </c>
       <c r="X173" s="7"/>
     </row>
-    <row r="174" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A174" s="4" t="s">
         <v>477</v>
       </c>
@@ -22766,7 +22799,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="190" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A190" s="4" t="s">
         <v>484</v>
       </c>
@@ -22839,7 +22872,7 @@
       </c>
       <c r="X190" s="7"/>
     </row>
-    <row r="191" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A191" s="4" t="s">
         <v>307</v>
       </c>
@@ -22912,7 +22945,7 @@
       </c>
       <c r="X191" s="7"/>
     </row>
-    <row r="192" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A192" s="4" t="s">
         <v>318</v>
       </c>
@@ -22985,7 +23018,7 @@
       </c>
       <c r="X192" s="7"/>
     </row>
-    <row r="193" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A193" s="4" t="s">
         <v>339</v>
       </c>
@@ -23058,7 +23091,7 @@
       </c>
       <c r="X193" s="7"/>
     </row>
-    <row r="194" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A194" s="4" t="s">
         <v>485</v>
       </c>
@@ -23131,7 +23164,7 @@
       </c>
       <c r="X194" s="7"/>
     </row>
-    <row r="195" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A195" s="4" t="s">
         <v>486</v>
       </c>
@@ -23204,7 +23237,7 @@
       </c>
       <c r="X195" s="7"/>
     </row>
-    <row r="196" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A196" s="4" t="s">
         <v>487</v>
       </c>
@@ -23277,7 +23310,7 @@
       </c>
       <c r="X196" s="7"/>
     </row>
-    <row r="197" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A197" s="4" t="s">
         <v>491</v>
       </c>
@@ -24475,7 +24508,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="213" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A213" s="4" t="s">
         <v>496</v>
       </c>
@@ -24548,7 +24581,7 @@
       </c>
       <c r="X213" s="7"/>
     </row>
-    <row r="214" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A214" s="4" t="s">
         <v>505</v>
       </c>
@@ -24621,7 +24654,7 @@
       </c>
       <c r="X214" s="7"/>
     </row>
-    <row r="215" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A215" s="4" t="s">
         <v>506</v>
       </c>
@@ -24694,7 +24727,7 @@
       </c>
       <c r="X215" s="7"/>
     </row>
-    <row r="216" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A216" s="4" t="s">
         <v>507</v>
       </c>
@@ -24767,7 +24800,7 @@
       </c>
       <c r="X216" s="7"/>
     </row>
-    <row r="217" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A217" s="4" t="s">
         <v>508</v>
       </c>
@@ -24840,7 +24873,7 @@
       </c>
       <c r="X217" s="7"/>
     </row>
-    <row r="218" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A218" s="4" t="s">
         <v>403</v>
       </c>
@@ -24913,7 +24946,7 @@
       </c>
       <c r="X218" s="7"/>
     </row>
-    <row r="219" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A219" s="4" t="s">
         <v>509</v>
       </c>
@@ -24986,7 +25019,7 @@
       </c>
       <c r="X219" s="7"/>
     </row>
-    <row r="220" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A220" s="4" t="s">
         <v>470</v>
       </c>
@@ -25059,7 +25092,7 @@
       </c>
       <c r="X220" s="7"/>
     </row>
-    <row r="221" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A221" s="4" t="s">
         <v>475</v>
       </c>
@@ -25132,7 +25165,7 @@
       </c>
       <c r="X221" s="7"/>
     </row>
-    <row r="222" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A222" s="4" t="s">
         <v>476</v>
       </c>
@@ -25205,7 +25238,7 @@
       </c>
       <c r="X222" s="7"/>
     </row>
-    <row r="223" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A223" s="4" t="s">
         <v>477</v>
       </c>
@@ -25278,7 +25311,7 @@
       </c>
       <c r="X223" s="7"/>
     </row>
-    <row r="224" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A224" s="4" t="s">
         <v>468</v>
       </c>
@@ -25351,7 +25384,7 @@
       </c>
       <c r="X224" s="7"/>
     </row>
-    <row r="225" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A225" s="4" t="s">
         <v>510</v>
       </c>
@@ -25424,7 +25457,7 @@
       </c>
       <c r="X225" s="7"/>
     </row>
-    <row r="226" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A226" s="4" t="s">
         <v>415</v>
       </c>
@@ -25497,7 +25530,7 @@
       </c>
       <c r="X226" s="7"/>
     </row>
-    <row r="227" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A227" s="4" t="s">
         <v>511</v>
       </c>
@@ -25570,7 +25603,7 @@
       </c>
       <c r="X227" s="7"/>
     </row>
-    <row r="228" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A228" s="4" t="s">
         <v>417</v>
       </c>
@@ -25643,7 +25676,7 @@
       </c>
       <c r="X228" s="7"/>
     </row>
-    <row r="229" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A229" s="4" t="s">
         <v>512</v>
       </c>
@@ -25716,7 +25749,7 @@
       </c>
       <c r="X229" s="7"/>
     </row>
-    <row r="230" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A230" s="4" t="s">
         <v>513</v>
       </c>
@@ -25789,7 +25822,7 @@
       </c>
       <c r="X230" s="7"/>
     </row>
-    <row r="231" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A231" s="4" t="s">
         <v>418</v>
       </c>
@@ -25862,7 +25895,7 @@
       </c>
       <c r="X231" s="7"/>
     </row>
-    <row r="232" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A232" s="4" t="s">
         <v>514</v>
       </c>
@@ -25935,7 +25968,7 @@
       </c>
       <c r="X232" s="7"/>
     </row>
-    <row r="233" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A233" s="4" t="s">
         <v>515</v>
       </c>
@@ -26008,7 +26041,7 @@
       </c>
       <c r="X233" s="7"/>
     </row>
-    <row r="234" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A234" s="4" t="s">
         <v>516</v>
       </c>
@@ -26081,7 +26114,7 @@
       </c>
       <c r="X234" s="7"/>
     </row>
-    <row r="235" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A235" s="4" t="s">
         <v>517</v>
       </c>
@@ -26154,7 +26187,7 @@
       </c>
       <c r="X235" s="7"/>
     </row>
-    <row r="236" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A236" s="4" t="s">
         <v>518</v>
       </c>
@@ -26227,7 +26260,7 @@
       </c>
       <c r="X236" s="7"/>
     </row>
-    <row r="237" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A237" s="4" t="s">
         <v>514</v>
       </c>
@@ -26300,7 +26333,7 @@
       </c>
       <c r="X237" s="7"/>
     </row>
-    <row r="238" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A238" s="4" t="s">
         <v>514</v>
       </c>
@@ -26373,7 +26406,7 @@
       </c>
       <c r="X238" s="7"/>
     </row>
-    <row r="239" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A239" s="4" t="s">
         <v>519</v>
       </c>
@@ -26446,7 +26479,7 @@
       </c>
       <c r="X239" s="7"/>
     </row>
-    <row r="240" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A240" s="4" t="s">
         <v>423</v>
       </c>
@@ -26594,7 +26627,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="242" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A242" s="4" t="s">
         <v>425</v>
       </c>
@@ -26892,7 +26925,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="246" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A246" s="4" t="s">
         <v>523</v>
       </c>
@@ -27115,7 +27148,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="249" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A249" s="4" t="s">
         <v>526</v>
       </c>
@@ -27188,7 +27221,7 @@
       </c>
       <c r="X249" s="7"/>
     </row>
-    <row r="250" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A250" s="4" t="s">
         <v>527</v>
       </c>
@@ -27261,7 +27294,7 @@
       </c>
       <c r="X250" s="7"/>
     </row>
-    <row r="251" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A251" s="4" t="s">
         <v>467</v>
       </c>
@@ -27334,7 +27367,7 @@
       </c>
       <c r="X251" s="7"/>
     </row>
-    <row r="252" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A252" s="4" t="s">
         <v>466</v>
       </c>
@@ -27557,7 +27590,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="255" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A255" s="4" t="s">
         <v>479</v>
       </c>
@@ -27705,7 +27738,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="257" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A257" s="4" t="s">
         <v>498</v>
       </c>
@@ -27778,7 +27811,7 @@
       </c>
       <c r="X257" s="7"/>
     </row>
-    <row r="258" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A258" s="4" t="s">
         <v>329</v>
       </c>
@@ -27851,7 +27884,7 @@
       </c>
       <c r="X258" s="7"/>
     </row>
-    <row r="259" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A259" s="4" t="s">
         <v>329</v>
       </c>
@@ -27924,7 +27957,7 @@
       </c>
       <c r="X259" s="7"/>
     </row>
-    <row r="260" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A260" s="4" t="s">
         <v>346</v>
       </c>
@@ -27997,7 +28030,7 @@
       </c>
       <c r="X260" s="7"/>
     </row>
-    <row r="261" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A261" s="4" t="s">
         <v>460</v>
       </c>
@@ -28070,7 +28103,7 @@
       </c>
       <c r="X261" s="7"/>
     </row>
-    <row r="262" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A262" s="4" t="s">
         <v>528</v>
       </c>
@@ -28143,7 +28176,7 @@
       </c>
       <c r="X262" s="7"/>
     </row>
-    <row r="263" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A263" s="4" t="s">
         <v>529</v>
       </c>
@@ -28216,7 +28249,7 @@
       </c>
       <c r="X263" s="7"/>
     </row>
-    <row r="264" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A264" s="4" t="s">
         <v>461</v>
       </c>
@@ -28289,7 +28322,7 @@
       </c>
       <c r="X264" s="7"/>
     </row>
-    <row r="265" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A265" s="4" t="s">
         <v>455</v>
       </c>
@@ -28362,7 +28395,7 @@
       </c>
       <c r="X265" s="7"/>
     </row>
-    <row r="266" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A266" s="4" t="s">
         <v>530</v>
       </c>
@@ -28435,7 +28468,7 @@
       </c>
       <c r="X266" s="7"/>
     </row>
-    <row r="267" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A267" s="4" t="s">
         <v>531</v>
       </c>
@@ -28508,7 +28541,7 @@
       </c>
       <c r="X267" s="7"/>
     </row>
-    <row r="268" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A268" s="4" t="s">
         <v>379</v>
       </c>
@@ -28581,7 +28614,7 @@
       </c>
       <c r="X268" s="7"/>
     </row>
-    <row r="269" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A269" s="4" t="s">
         <v>377</v>
       </c>
@@ -28654,7 +28687,7 @@
       </c>
       <c r="X269" s="7"/>
     </row>
-    <row r="270" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A270" s="4" t="s">
         <v>409</v>
       </c>
@@ -28727,7 +28760,7 @@
       </c>
       <c r="X270" s="7"/>
     </row>
-    <row r="271" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A271" s="4" t="s">
         <v>315</v>
       </c>
@@ -28800,7 +28833,7 @@
       </c>
       <c r="X271" s="7"/>
     </row>
-    <row r="272" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A272" s="4" t="s">
         <v>533</v>
       </c>
@@ -28873,7 +28906,7 @@
       </c>
       <c r="X272" s="7"/>
     </row>
-    <row r="273" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A273" s="4" t="s">
         <v>535</v>
       </c>
@@ -28946,7 +28979,7 @@
       </c>
       <c r="X273" s="7"/>
     </row>
-    <row r="274" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A274" s="4" t="s">
         <v>536</v>
       </c>
@@ -29019,7 +29052,7 @@
       </c>
       <c r="X274" s="7"/>
     </row>
-    <row r="275" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A275" s="4" t="s">
         <v>538</v>
       </c>
@@ -29092,7 +29125,7 @@
       </c>
       <c r="X275" s="7"/>
     </row>
-    <row r="276" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A276" s="4" t="s">
         <v>539</v>
       </c>
@@ -29165,7 +29198,7 @@
       </c>
       <c r="X276" s="7"/>
     </row>
-    <row r="277" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A277" s="4" t="s">
         <v>540</v>
       </c>
@@ -31563,7 +31596,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="309" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A309" s="4" t="s">
         <v>472</v>
       </c>
@@ -31861,7 +31894,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="313" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A313" s="4" t="s">
         <v>507</v>
       </c>
@@ -31934,7 +31967,7 @@
       </c>
       <c r="X313" s="7"/>
     </row>
-    <row r="314" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A314" s="4" t="s">
         <v>556</v>
       </c>
@@ -32007,7 +32040,7 @@
       </c>
       <c r="X314" s="7"/>
     </row>
-    <row r="315" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A315" s="4" t="s">
         <v>557</v>
       </c>
@@ -32080,7 +32113,7 @@
       </c>
       <c r="X315" s="7"/>
     </row>
-    <row r="316" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A316" s="4" t="s">
         <v>560</v>
       </c>
@@ -32153,7 +32186,7 @@
       </c>
       <c r="X316" s="7"/>
     </row>
-    <row r="317" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A317" s="4" t="s">
         <v>561</v>
       </c>
@@ -32226,7 +32259,7 @@
       </c>
       <c r="X317" s="7"/>
     </row>
-    <row r="318" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A318" s="4" t="s">
         <v>562</v>
       </c>
@@ -32299,7 +32332,7 @@
       </c>
       <c r="X318" s="7"/>
     </row>
-    <row r="319" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A319" s="4" t="s">
         <v>563</v>
       </c>
@@ -32372,7 +32405,7 @@
       </c>
       <c r="X319" s="7"/>
     </row>
-    <row r="320" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A320" s="4" t="s">
         <v>564</v>
       </c>
@@ -32445,7 +32478,7 @@
       </c>
       <c r="X320" s="7"/>
     </row>
-    <row r="321" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A321" s="4" t="s">
         <v>565</v>
       </c>
@@ -32518,7 +32551,7 @@
       </c>
       <c r="X321" s="7"/>
     </row>
-    <row r="322" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A322" s="4" t="s">
         <v>566</v>
       </c>
@@ -32591,7 +32624,7 @@
       </c>
       <c r="X322" s="7"/>
     </row>
-    <row r="323" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A323" s="4" t="s">
         <v>567</v>
       </c>
@@ -32664,7 +32697,7 @@
       </c>
       <c r="X323" s="7"/>
     </row>
-    <row r="324" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A324" s="4" t="s">
         <v>568</v>
       </c>
@@ -32737,7 +32770,7 @@
       </c>
       <c r="X324" s="7"/>
     </row>
-    <row r="325" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A325" s="4" t="s">
         <v>569</v>
       </c>
@@ -32810,7 +32843,7 @@
       </c>
       <c r="X325" s="7"/>
     </row>
-    <row r="326" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A326" s="4" t="s">
         <v>570</v>
       </c>
@@ -32883,7 +32916,7 @@
       </c>
       <c r="X326" s="7"/>
     </row>
-    <row r="327" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A327" s="4" t="s">
         <v>571</v>
       </c>
@@ -32956,7 +32989,7 @@
       </c>
       <c r="X327" s="7"/>
     </row>
-    <row r="328" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A328" s="4" t="s">
         <v>515</v>
       </c>
@@ -33029,7 +33062,7 @@
       </c>
       <c r="X328" s="7"/>
     </row>
-    <row r="329" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A329" s="4" t="s">
         <v>518</v>
       </c>
@@ -33102,7 +33135,7 @@
       </c>
       <c r="X329" s="7"/>
     </row>
-    <row r="330" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A330" s="4" t="s">
         <v>573</v>
       </c>
@@ -33175,7 +33208,7 @@
       </c>
       <c r="X330" s="7"/>
     </row>
-    <row r="331" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A331" s="4" t="s">
         <v>574</v>
       </c>
@@ -33248,7 +33281,7 @@
       </c>
       <c r="X331" s="7"/>
     </row>
-    <row r="332" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A332" s="4" t="s">
         <v>401</v>
       </c>
@@ -33396,7 +33429,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="334" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A334" s="4" t="s">
         <v>379</v>
       </c>
@@ -33469,7 +33502,7 @@
       </c>
       <c r="X334" s="7"/>
     </row>
-    <row r="335" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A335" s="4" t="s">
         <v>577</v>
       </c>
@@ -33542,7 +33575,7 @@
       </c>
       <c r="X335" s="7"/>
     </row>
-    <row r="336" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A336" s="4" t="s">
         <v>579</v>
       </c>
@@ -33615,7 +33648,7 @@
       </c>
       <c r="X336" s="7"/>
     </row>
-    <row r="337" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A337" s="4" t="s">
         <v>580</v>
       </c>
@@ -33688,7 +33721,7 @@
       </c>
       <c r="X337" s="7"/>
     </row>
-    <row r="338" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A338" s="4" t="s">
         <v>581</v>
       </c>
@@ -33761,7 +33794,7 @@
       </c>
       <c r="X338" s="7"/>
     </row>
-    <row r="339" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A339" s="4" t="s">
         <v>582</v>
       </c>
@@ -33834,7 +33867,7 @@
       </c>
       <c r="X339" s="7"/>
     </row>
-    <row r="340" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A340" s="4" t="s">
         <v>584</v>
       </c>
@@ -33907,7 +33940,7 @@
       </c>
       <c r="X340" s="7"/>
     </row>
-    <row r="341" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A341" s="4" t="s">
         <v>460</v>
       </c>
@@ -33980,7 +34013,7 @@
       </c>
       <c r="X341" s="7"/>
     </row>
-    <row r="342" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A342" s="4" t="s">
         <v>585</v>
       </c>
@@ -36528,7 +36561,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="376" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A376" s="4" t="s">
         <v>470</v>
       </c>
@@ -36601,7 +36634,7 @@
       </c>
       <c r="X376" s="7"/>
     </row>
-    <row r="377" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A377" s="4" t="s">
         <v>411</v>
       </c>
@@ -36674,7 +36707,7 @@
       </c>
       <c r="X377" s="7"/>
     </row>
-    <row r="378" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A378" s="4" t="s">
         <v>598</v>
       </c>
@@ -36747,7 +36780,7 @@
       </c>
       <c r="X378" s="7"/>
     </row>
-    <row r="379" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A379" s="4" t="s">
         <v>599</v>
       </c>
@@ -36820,7 +36853,7 @@
       </c>
       <c r="X379" s="7"/>
     </row>
-    <row r="380" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A380" s="4" t="s">
         <v>600</v>
       </c>
@@ -36893,7 +36926,7 @@
       </c>
       <c r="X380" s="7"/>
     </row>
-    <row r="381" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A381" s="4" t="s">
         <v>602</v>
       </c>
@@ -36966,7 +36999,7 @@
       </c>
       <c r="X381" s="7"/>
     </row>
-    <row r="382" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A382" s="4" t="s">
         <v>603</v>
       </c>
@@ -37039,7 +37072,7 @@
       </c>
       <c r="X382" s="7"/>
     </row>
-    <row r="383" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A383" s="4" t="s">
         <v>604</v>
       </c>
@@ -37112,7 +37145,7 @@
       </c>
       <c r="X383" s="7"/>
     </row>
-    <row r="384" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A384" s="4" t="s">
         <v>605</v>
       </c>
@@ -37185,7 +37218,7 @@
       </c>
       <c r="X384" s="7"/>
     </row>
-    <row r="385" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A385" s="4" t="s">
         <v>606</v>
       </c>
@@ -37258,7 +37291,7 @@
       </c>
       <c r="X385" s="7"/>
     </row>
-    <row r="386" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A386" s="4" t="s">
         <v>607</v>
       </c>
@@ -37331,7 +37364,7 @@
       </c>
       <c r="X386" s="7"/>
     </row>
-    <row r="387" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A387" s="4" t="s">
         <v>608</v>
       </c>
@@ -37404,7 +37437,7 @@
       </c>
       <c r="X387" s="7"/>
     </row>
-    <row r="388" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A388" s="4" t="s">
         <v>609</v>
       </c>
@@ -37477,7 +37510,7 @@
       </c>
       <c r="X388" s="7"/>
     </row>
-    <row r="389" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A389" s="4" t="s">
         <v>610</v>
       </c>
@@ -37550,7 +37583,7 @@
       </c>
       <c r="X389" s="7"/>
     </row>
-    <row r="390" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A390" s="4" t="s">
         <v>610</v>
       </c>
@@ -37623,7 +37656,7 @@
       </c>
       <c r="X390" s="7"/>
     </row>
-    <row r="391" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A391" s="4" t="s">
         <v>612</v>
       </c>
@@ -37696,7 +37729,7 @@
       </c>
       <c r="X391" s="7"/>
     </row>
-    <row r="392" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A392" s="4" t="s">
         <v>613</v>
       </c>
@@ -37769,7 +37802,7 @@
       </c>
       <c r="X392" s="7"/>
     </row>
-    <row r="393" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A393" s="4" t="s">
         <v>606</v>
       </c>
@@ -37842,7 +37875,7 @@
       </c>
       <c r="X393" s="7"/>
     </row>
-    <row r="394" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A394" s="4" t="s">
         <v>607</v>
       </c>
@@ -37915,7 +37948,7 @@
       </c>
       <c r="X394" s="7"/>
     </row>
-    <row r="395" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A395" s="4" t="s">
         <v>604</v>
       </c>
@@ -37988,7 +38021,7 @@
       </c>
       <c r="X395" s="7"/>
     </row>
-    <row r="396" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A396" s="4" t="s">
         <v>415</v>
       </c>
@@ -38061,7 +38094,7 @@
       </c>
       <c r="X396" s="7"/>
     </row>
-    <row r="397" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A397" s="4" t="s">
         <v>608</v>
       </c>
@@ -38134,7 +38167,7 @@
       </c>
       <c r="X397" s="7"/>
     </row>
-    <row r="398" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A398" s="4" t="s">
         <v>609</v>
       </c>
@@ -38207,7 +38240,7 @@
       </c>
       <c r="X398" s="7"/>
     </row>
-    <row r="399" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A399" s="4" t="s">
         <v>605</v>
       </c>
@@ -38280,7 +38313,7 @@
       </c>
       <c r="X399" s="7"/>
     </row>
-    <row r="400" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A400" s="4" t="s">
         <v>605</v>
       </c>
@@ -38353,7 +38386,7 @@
       </c>
       <c r="X400" s="7"/>
     </row>
-    <row r="401" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A401" s="4" t="s">
         <v>605</v>
       </c>
@@ -38426,7 +38459,7 @@
       </c>
       <c r="X401" s="7"/>
     </row>
-    <row r="402" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A402" s="4" t="s">
         <v>418</v>
       </c>
@@ -38499,7 +38532,7 @@
       </c>
       <c r="X402" s="7"/>
     </row>
-    <row r="403" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A403" s="4" t="s">
         <v>615</v>
       </c>
@@ -38572,7 +38605,7 @@
       </c>
       <c r="X403" s="7"/>
     </row>
-    <row r="404" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A404" s="4" t="s">
         <v>616</v>
       </c>
@@ -38645,7 +38678,7 @@
       </c>
       <c r="X404" s="7"/>
     </row>
-    <row r="405" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A405" s="4" t="s">
         <v>617</v>
       </c>
@@ -38718,7 +38751,7 @@
       </c>
       <c r="X405" s="7"/>
     </row>
-    <row r="406" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A406" s="4" t="s">
         <v>618</v>
       </c>
@@ -38791,7 +38824,7 @@
       </c>
       <c r="X406" s="7"/>
     </row>
-    <row r="407" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A407" s="4" t="s">
         <v>404</v>
       </c>
@@ -38864,7 +38897,7 @@
       </c>
       <c r="X407" s="7"/>
     </row>
-    <row r="408" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A408" s="4" t="s">
         <v>619</v>
       </c>
@@ -38937,7 +38970,7 @@
       </c>
       <c r="X408" s="7"/>
     </row>
-    <row r="409" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A409" s="4" t="s">
         <v>620</v>
       </c>
@@ -39010,7 +39043,7 @@
       </c>
       <c r="X409" s="7"/>
     </row>
-    <row r="410" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A410" s="4" t="s">
         <v>474</v>
       </c>
@@ -39083,7 +39116,7 @@
       </c>
       <c r="X410" s="7"/>
     </row>
-    <row r="411" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A411" s="4" t="s">
         <v>368</v>
       </c>
@@ -39156,7 +39189,7 @@
       </c>
       <c r="X411" s="7"/>
     </row>
-    <row r="412" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A412" s="4" t="s">
         <v>623</v>
       </c>
@@ -39229,7 +39262,7 @@
       </c>
       <c r="X412" s="7"/>
     </row>
-    <row r="413" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A413" s="4" t="s">
         <v>335</v>
       </c>
@@ -39302,7 +39335,7 @@
       </c>
       <c r="X413" s="7"/>
     </row>
-    <row r="414" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A414" s="4" t="s">
         <v>345</v>
       </c>
@@ -39375,7 +39408,7 @@
       </c>
       <c r="X414" s="7"/>
     </row>
-    <row r="415" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A415" s="4" t="s">
         <v>464</v>
       </c>
@@ -39448,7 +39481,7 @@
       </c>
       <c r="X415" s="7"/>
     </row>
-    <row r="416" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A416" s="4" t="s">
         <v>624</v>
       </c>
@@ -39521,7 +39554,7 @@
       </c>
       <c r="X416" s="7"/>
     </row>
-    <row r="417" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A417" s="4" t="s">
         <v>625</v>
       </c>
@@ -39594,7 +39627,7 @@
       </c>
       <c r="X417" s="7"/>
     </row>
-    <row r="418" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A418" s="4" t="s">
         <v>462</v>
       </c>
@@ -39667,7 +39700,7 @@
       </c>
       <c r="X418" s="7"/>
     </row>
-    <row r="419" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A419" s="4" t="s">
         <v>626</v>
       </c>
@@ -39740,7 +39773,7 @@
       </c>
       <c r="X419" s="7"/>
     </row>
-    <row r="420" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A420" s="4" t="s">
         <v>627</v>
       </c>
@@ -39813,7 +39846,7 @@
       </c>
       <c r="X420" s="7"/>
     </row>
-    <row r="421" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A421" s="4" t="s">
         <v>629</v>
       </c>
@@ -39886,7 +39919,7 @@
       </c>
       <c r="X421" s="7"/>
     </row>
-    <row r="422" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A422" s="4" t="s">
         <v>630</v>
       </c>
@@ -39959,7 +39992,7 @@
       </c>
       <c r="X422" s="7"/>
     </row>
-    <row r="423" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A423" s="4" t="s">
         <v>631</v>
       </c>
@@ -40032,7 +40065,7 @@
       </c>
       <c r="X423" s="7"/>
     </row>
-    <row r="424" spans="1:24" hidden="1" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A424" s="4" t="s">
         <v>446</v>
       </c>
@@ -41461,4 +41494,403 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1EB5DAB-8040-4436-8720-598F8C35D45F}">
+  <dimension ref="A1:D29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U19" sqref="U19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.21875" style="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
+        <v>667</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>664</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="15">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>60.410000000000004</v>
+      </c>
+      <c r="C2">
+        <v>-28.660229999999999</v>
+      </c>
+      <c r="D2">
+        <v>21.138770000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="15">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>48.3</v>
+      </c>
+      <c r="C3">
+        <v>-28.66422</v>
+      </c>
+      <c r="D3">
+        <v>21.13672</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="15">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>52.019999999999996</v>
+      </c>
+      <c r="C4">
+        <v>-28.431609999999999</v>
+      </c>
+      <c r="D4">
+        <v>20.659839999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="15">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>42.96</v>
+      </c>
+      <c r="C5">
+        <v>-28.653279999999999</v>
+      </c>
+      <c r="D5">
+        <v>21.156929999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="15">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>32.339999999999996</v>
+      </c>
+      <c r="C6">
+        <v>-28.657769999999999</v>
+      </c>
+      <c r="D6">
+        <v>21.125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="15">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>61.440000000000005</v>
+      </c>
+      <c r="C7">
+        <v>-28.461099999999998</v>
+      </c>
+      <c r="D7">
+        <v>20.659610000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="15">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>13.35</v>
+      </c>
+      <c r="C8">
+        <v>-28.805540000000001</v>
+      </c>
+      <c r="D8">
+        <v>20.653639999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="15">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>37.729999999999997</v>
+      </c>
+      <c r="C9">
+        <v>-28.494689999999999</v>
+      </c>
+      <c r="D9">
+        <v>20.14799</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="15">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>29.47</v>
+      </c>
+      <c r="C10">
+        <v>-28.430779999999999</v>
+      </c>
+      <c r="D10">
+        <v>20.140129999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="15">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>42.585000000000001</v>
+      </c>
+      <c r="C11">
+        <v>-28.6542037</v>
+      </c>
+      <c r="D11">
+        <v>19.5236904</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="15">
+        <v>16</v>
+      </c>
+      <c r="B12">
+        <v>49.273000000000003</v>
+      </c>
+      <c r="C12">
+        <v>-28.6542037</v>
+      </c>
+      <c r="D12">
+        <v>19.5236904</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="15">
+        <v>18</v>
+      </c>
+      <c r="B13">
+        <v>46.85</v>
+      </c>
+      <c r="C13">
+        <v>-28.6542037</v>
+      </c>
+      <c r="D13">
+        <v>19.5236904</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="15">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>45.11</v>
+      </c>
+      <c r="C14">
+        <v>-28.6542037</v>
+      </c>
+      <c r="D14">
+        <v>19.5236904</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="15">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>47.78</v>
+      </c>
+      <c r="C15">
+        <v>-28.6542037</v>
+      </c>
+      <c r="D15">
+        <v>21.112120000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="15">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>43.750000000000014</v>
+      </c>
+      <c r="C16">
+        <v>-28.6542037</v>
+      </c>
+      <c r="D16">
+        <v>19.5236904</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="15">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>40.380000000000003</v>
+      </c>
+      <c r="C17">
+        <v>-28.958385499999999</v>
+      </c>
+      <c r="D17">
+        <v>19.000456199999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="15">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>44.849999999999994</v>
+      </c>
+      <c r="C18">
+        <v>-28.958385499999999</v>
+      </c>
+      <c r="D18">
+        <v>19.000456199999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="15">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <v>15.04</v>
+      </c>
+      <c r="C19">
+        <v>-28.958385499999999</v>
+      </c>
+      <c r="D19">
+        <v>19.000456199999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="15">
+        <v>31</v>
+      </c>
+      <c r="B20">
+        <v>59.07</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="15">
+        <v>43</v>
+      </c>
+      <c r="B21">
+        <v>51.480000000000004</v>
+      </c>
+      <c r="C21">
+        <v>-28.653929999999999</v>
+      </c>
+      <c r="D21">
+        <v>21.111249999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="15">
+        <v>44</v>
+      </c>
+      <c r="B22">
+        <v>100.33999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="15">
+        <v>45</v>
+      </c>
+      <c r="B23">
+        <v>61.84</v>
+      </c>
+      <c r="C23">
+        <v>-28.663430000000002</v>
+      </c>
+      <c r="D23">
+        <v>21.157830000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="15">
+        <v>46</v>
+      </c>
+      <c r="B24">
+        <v>55.41</v>
+      </c>
+      <c r="C24">
+        <v>-28.668130000000001</v>
+      </c>
+      <c r="D24">
+        <v>21.151949999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="15">
+        <v>47</v>
+      </c>
+      <c r="B25">
+        <v>61.79999999999999</v>
+      </c>
+      <c r="C25">
+        <v>-28.654140000000002</v>
+      </c>
+      <c r="D25">
+        <v>21.15917</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="15">
+        <v>73</v>
+      </c>
+      <c r="B26">
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <v>-28.65372</v>
+      </c>
+      <c r="D26">
+        <v>21.114560000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="15">
+        <v>74</v>
+      </c>
+      <c r="B27">
+        <v>71.789999999999992</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="15">
+        <v>75</v>
+      </c>
+      <c r="B28">
+        <v>40.620000000000005</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="15">
+        <v>76</v>
+      </c>
+      <c r="B29">
+        <v>60.61</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D29" xr:uid="{4F42FAB1-4A78-40D5-9FA1-8979E0D3CE99}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D29">
+      <sortCondition ref="A1:A29"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updates to data model to pull real data from database
</commit_message>
<xml_diff>
--- a/input_data/oc_site.xlsx
+++ b/input_data/oc_site.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jolene\GoogleDrive\Personal\Study\phd\model\workdir\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE700677-7BC4-4DF1-9A00-0AE549725E57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{916D3408-483A-4F5B-BB6E-1DD0E52B89D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="3" xr2:uid="{6FE78FDE-FEA8-4741-9142-6B1CDDCD843D}"/>
+    <workbookView xWindow="60" yWindow="660" windowWidth="17280" windowHeight="9060" firstSheet="2" activeTab="3" xr2:uid="{6FE78FDE-FEA8-4741-9142-6B1CDDCD843D}"/>
   </bookViews>
   <sheets>
     <sheet name="sites" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="oc_site" sheetId="2" state="hidden" r:id="rId2"/>
     <sheet name="oc" sheetId="3" r:id="rId3"/>
-    <sheet name="pu" sheetId="4" r:id="rId4"/>
+    <sheet name="pu" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">oc!$A$1:$T$443</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">oc_site!$A$1:$H$186</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">pu!$A$1:$D$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">pu!$A$1:$D$38</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">sites!$A$1:$D$44</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -2136,7 +2136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2157,6 +2157,9 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -41497,11 +41500,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1EB5DAB-8040-4436-8720-598F8C35D45F}">
-  <dimension ref="A1:D29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8BBF130-4CD6-4BEB-986E-6B2F495348EB}">
+  <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U19" sqref="U19"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -41553,150 +41556,147 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>52.019999999999996</v>
+        <v>73</v>
       </c>
       <c r="C4">
-        <v>-28.431609999999999</v>
+        <v>-28.780999999999999</v>
       </c>
       <c r="D4">
-        <v>20.659839999999999</v>
+        <v>20.780999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>42.96</v>
+        <v>52.019999999999996</v>
       </c>
       <c r="C5">
-        <v>-28.653279999999999</v>
+        <v>-28.431609999999999</v>
       </c>
       <c r="D5">
-        <v>21.156929999999999</v>
+        <v>20.659839999999999</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>32.339999999999996</v>
+        <v>42.96</v>
       </c>
       <c r="C6">
-        <v>-28.657769999999999</v>
+        <v>-28.653279999999999</v>
       </c>
       <c r="D6">
-        <v>21.125</v>
+        <v>21.156929999999999</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="15">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>61.440000000000005</v>
+        <v>32.339999999999996</v>
       </c>
       <c r="C7">
-        <v>-28.461099999999998</v>
+        <v>-28.657769999999999</v>
       </c>
       <c r="D7">
-        <v>20.659610000000001</v>
+        <v>21.125</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="15">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>13.35</v>
+        <v>61.440000000000005</v>
       </c>
       <c r="C8">
-        <v>-28.805540000000001</v>
+        <v>-28.461099999999998</v>
       </c>
       <c r="D8">
-        <v>20.653639999999999</v>
+        <v>20.659610000000001</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="15">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>37.729999999999997</v>
+        <v>13.35</v>
       </c>
       <c r="C9">
-        <v>-28.494689999999999</v>
+        <v>-28.805540000000001</v>
       </c>
       <c r="D9">
-        <v>20.14799</v>
+        <v>20.653639999999999</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="15">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>29.47</v>
+        <v>100.27</v>
       </c>
       <c r="C10">
-        <v>-28.430779999999999</v>
+        <v>-28.498000000000001</v>
       </c>
       <c r="D10">
-        <v>20.140129999999999</v>
+        <v>20.143999999999998</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="15">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>42.585000000000001</v>
+        <v>37.729999999999997</v>
       </c>
       <c r="C11">
-        <v>-28.6542037</v>
+        <v>-28.494689999999999</v>
       </c>
       <c r="D11">
-        <v>19.5236904</v>
+        <v>20.14799</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="15">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>49.273000000000003</v>
+        <v>29.47</v>
       </c>
       <c r="C12">
-        <v>-28.6542037</v>
+        <v>-28.430779999999999</v>
       </c>
       <c r="D12">
-        <v>19.5236904</v>
+        <v>20.140129999999999</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="15">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>46.85</v>
+        <v>100</v>
       </c>
       <c r="C13">
-        <v>-28.6542037</v>
+        <v>-28.454999999999998</v>
       </c>
       <c r="D13">
-        <v>19.5236904</v>
+        <v>20.044</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="15">
-        <v>21</v>
-      </c>
-      <c r="B14">
-        <v>45.11</v>
+        <v>14</v>
       </c>
       <c r="C14">
         <v>-28.6542037</v>
@@ -41707,24 +41707,24 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="15">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="B15">
-        <v>47.78</v>
+        <v>42.585000000000001</v>
       </c>
       <c r="C15">
         <v>-28.6542037</v>
       </c>
       <c r="D15">
-        <v>21.112120000000001</v>
+        <v>19.5236904</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="15">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="B16">
-        <v>43.750000000000014</v>
+        <v>49.273000000000003</v>
       </c>
       <c r="C16">
         <v>-28.6542037</v>
@@ -41735,162 +41735,534 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="15">
-        <v>24</v>
-      </c>
-      <c r="B17">
-        <v>40.380000000000003</v>
+        <v>17</v>
       </c>
       <c r="C17">
-        <v>-28.958385499999999</v>
+        <v>-28.6542037</v>
       </c>
       <c r="D17">
-        <v>19.000456199999999</v>
+        <v>19.5236904</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="15">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B18">
-        <v>44.849999999999994</v>
+        <v>46.85</v>
       </c>
       <c r="C18">
-        <v>-28.958385499999999</v>
+        <v>-28.6542037</v>
       </c>
       <c r="D18">
-        <v>19.000456199999999</v>
+        <v>19.5236904</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="15">
-        <v>26</v>
-      </c>
-      <c r="B19">
-        <v>15.04</v>
+        <v>19</v>
       </c>
       <c r="C19">
-        <v>-28.958385499999999</v>
+        <v>-28.6542037</v>
       </c>
       <c r="D19">
-        <v>19.000456199999999</v>
+        <v>19.5236904</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="15">
-        <v>31</v>
-      </c>
-      <c r="B20">
-        <v>59.07</v>
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <v>-28.6542037</v>
+      </c>
+      <c r="D20">
+        <v>19.5236904</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="15">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="B21">
-        <v>51.480000000000004</v>
+        <v>45.11</v>
       </c>
       <c r="C21">
-        <v>-28.653929999999999</v>
+        <v>-28.6542037</v>
       </c>
       <c r="D21">
-        <v>21.111249999999998</v>
+        <v>19.5236904</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="15">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="B22">
-        <v>100.33999999999996</v>
+        <v>47.78</v>
+      </c>
+      <c r="C22">
+        <v>-28.6542037</v>
+      </c>
+      <c r="D22">
+        <v>21.112120000000001</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="15">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B23">
-        <v>61.84</v>
+        <v>43.750000000000014</v>
       </c>
       <c r="C23">
-        <v>-28.663430000000002</v>
+        <v>-28.6542037</v>
       </c>
       <c r="D23">
-        <v>21.157830000000001</v>
+        <v>19.5236904</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="15">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="B24">
-        <v>55.41</v>
+        <v>40.380000000000003</v>
       </c>
       <c r="C24">
-        <v>-28.668130000000001</v>
+        <v>-28.958385499999999</v>
       </c>
       <c r="D24">
-        <v>21.151949999999999</v>
+        <v>19.000456199999999</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="15">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="B25">
-        <v>61.79999999999999</v>
+        <v>44.849999999999994</v>
       </c>
       <c r="C25">
-        <v>-28.654140000000002</v>
+        <v>-28.958385499999999</v>
       </c>
       <c r="D25">
-        <v>21.15917</v>
+        <v>19.000456199999999</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="15">
-        <v>73</v>
+        <v>26</v>
       </c>
       <c r="B26">
-        <v>8</v>
+        <v>15.04</v>
       </c>
       <c r="C26">
-        <v>-28.65372</v>
+        <v>-28.958385499999999</v>
       </c>
       <c r="D26">
-        <v>21.114560000000001</v>
+        <v>19.000456199999999</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="15">
-        <v>74</v>
-      </c>
-      <c r="B27">
-        <v>71.789999999999992</v>
+        <v>27</v>
+      </c>
+      <c r="C27">
+        <v>-28.6542037</v>
+      </c>
+      <c r="D27">
+        <v>19.5236904</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="15">
-        <v>75</v>
-      </c>
-      <c r="B28">
-        <v>40.620000000000005</v>
+        <v>33</v>
+      </c>
+      <c r="C28">
+        <v>-34.076157000000002</v>
+      </c>
+      <c r="D28">
+        <v>18.892171000000001</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="15">
+        <v>43</v>
+      </c>
+      <c r="B29">
+        <v>51.480000000000004</v>
+      </c>
+      <c r="C29">
+        <v>-28.653929999999999</v>
+      </c>
+      <c r="D29">
+        <v>21.111249999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="15">
+        <v>44</v>
+      </c>
+      <c r="B30">
+        <v>100.33999999999996</v>
+      </c>
+      <c r="C30">
+        <v>-33.444966999999998</v>
+      </c>
+      <c r="D30">
+        <v>19.629231999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="15">
+        <v>45</v>
+      </c>
+      <c r="B31">
+        <v>61.84</v>
+      </c>
+      <c r="C31">
+        <v>-28.663430000000002</v>
+      </c>
+      <c r="D31">
+        <v>21.157830000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="15">
+        <v>46</v>
+      </c>
+      <c r="B32">
+        <v>55.41</v>
+      </c>
+      <c r="C32">
+        <v>-28.668130000000001</v>
+      </c>
+      <c r="D32">
+        <v>21.151949999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="15">
+        <v>47</v>
+      </c>
+      <c r="B33">
+        <v>61.79999999999999</v>
+      </c>
+      <c r="C33">
+        <v>-28.654140000000002</v>
+      </c>
+      <c r="D33">
+        <v>21.15917</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="15">
+        <v>48</v>
+      </c>
+      <c r="B34">
+        <v>66.14</v>
+      </c>
+      <c r="C34">
+        <v>-33.793973999999999</v>
+      </c>
+      <c r="D34">
+        <v>19.828016999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="15">
+        <v>73</v>
+      </c>
+      <c r="B35">
+        <v>8</v>
+      </c>
+      <c r="C35">
+        <v>-28.65372</v>
+      </c>
+      <c r="D35">
+        <v>21.114560000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="15">
+        <v>74</v>
+      </c>
+      <c r="B36">
+        <v>71.789999999999992</v>
+      </c>
+      <c r="C36">
+        <v>-32.901696999999999</v>
+      </c>
+      <c r="D36">
+        <v>18.746009000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="15">
+        <v>75</v>
+      </c>
+      <c r="B37">
+        <v>40.620000000000005</v>
+      </c>
+      <c r="C37">
+        <v>-33.793973999999999</v>
+      </c>
+      <c r="D37">
+        <v>19.828016999999999</v>
+      </c>
+      <c r="H37">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="15">
         <v>76</v>
       </c>
-      <c r="B29">
+      <c r="B38">
         <v>60.61</v>
       </c>
+      <c r="C38">
+        <v>-32.901696999999999</v>
+      </c>
+      <c r="D38">
+        <v>18.746009000000001</v>
+      </c>
+      <c r="H38">
+        <f>H37*60</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="16">
+        <v>93</v>
+      </c>
+      <c r="B39">
+        <v>114.86</v>
+      </c>
+      <c r="C39">
+        <v>-25.093</v>
+      </c>
+      <c r="D39">
+        <v>29.387</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="15">
+        <v>77</v>
+      </c>
+      <c r="C40">
+        <v>-28.6542037</v>
+      </c>
+      <c r="D40">
+        <v>19.5236904</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="15">
+        <v>78</v>
+      </c>
+      <c r="C41">
+        <v>-28.6542037</v>
+      </c>
+      <c r="D41">
+        <v>19.5236904</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="15">
+        <v>79</v>
+      </c>
+      <c r="C42">
+        <v>-28.6542037</v>
+      </c>
+      <c r="D42">
+        <v>19.5236904</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="15">
+        <v>80</v>
+      </c>
+      <c r="C43">
+        <v>-28.6542037</v>
+      </c>
+      <c r="D43">
+        <v>19.5236904</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" s="15">
+        <v>81</v>
+      </c>
+      <c r="C44">
+        <v>-28.6542037</v>
+      </c>
+      <c r="D44">
+        <v>19.5236904</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" s="15">
+        <v>82</v>
+      </c>
+      <c r="C45">
+        <v>-28.6542037</v>
+      </c>
+      <c r="D45">
+        <v>19.5236904</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="15">
+        <v>83</v>
+      </c>
+      <c r="C46">
+        <v>-28.6542037</v>
+      </c>
+      <c r="D46">
+        <v>19.5236904</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" s="15">
+        <v>84</v>
+      </c>
+      <c r="C47">
+        <v>-28.6542037</v>
+      </c>
+      <c r="D47">
+        <v>19.5236904</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" s="15">
+        <v>85</v>
+      </c>
+      <c r="C48">
+        <v>-28.6542037</v>
+      </c>
+      <c r="D48">
+        <v>19.5236904</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="15">
+        <v>68</v>
+      </c>
+      <c r="C49">
+        <v>-28.646999999999998</v>
+      </c>
+      <c r="D49">
+        <v>19.515000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="15">
+        <v>87</v>
+      </c>
+      <c r="C50">
+        <v>-28.646999999999998</v>
+      </c>
+      <c r="D50">
+        <v>19.515000000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="15">
+        <v>88</v>
+      </c>
+      <c r="C51">
+        <v>-28.646999999999998</v>
+      </c>
+      <c r="D51">
+        <v>19.515000000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="15">
+        <v>92</v>
+      </c>
+      <c r="C52" s="1">
+        <v>-28.660229999999999</v>
+      </c>
+      <c r="D52" s="1">
+        <v>21.138770000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="15">
+        <v>96</v>
+      </c>
+      <c r="C53">
+        <v>-25.093</v>
+      </c>
+      <c r="D53">
+        <v>29.387</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="15">
+        <v>55</v>
+      </c>
+      <c r="C54">
+        <v>-28.795000000000002</v>
+      </c>
+      <c r="D54">
+        <v>20.64</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="15">
+        <v>51</v>
+      </c>
+      <c r="C55">
+        <v>-28.795000000000002</v>
+      </c>
+      <c r="D55">
+        <v>20.64</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="15">
+        <v>52</v>
+      </c>
+      <c r="C56">
+        <v>-28.795000000000002</v>
+      </c>
+      <c r="D56">
+        <v>20.64</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="15">
+        <v>66</v>
+      </c>
+      <c r="C57">
+        <v>-28.795000000000002</v>
+      </c>
+      <c r="D57">
+        <v>20.64</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="15">
+        <v>69</v>
+      </c>
+      <c r="C58">
+        <v>-28.795000000000002</v>
+      </c>
+      <c r="D58">
+        <v>20.64</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D29" xr:uid="{4F42FAB1-4A78-40D5-9FA1-8979E0D3CE99}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D29">
-      <sortCondition ref="A1:A29"/>
+  <autoFilter ref="A1:D38" xr:uid="{4F42FAB1-4A78-40D5-9FA1-8979E0D3CE99}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D38">
+      <sortCondition ref="A1:A38"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>